<commit_message>
updated maps and code
</commit_message>
<xml_diff>
--- a/Results table.xlsx
+++ b/Results table.xlsx
@@ -4,16 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5460" yWindow="2080" windowWidth="27720" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="3500" yWindow="2200" windowWidth="27720" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
     <sheet name="CLT colour" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$E$104</definedName>
     <definedName name="cons_day_rate" localSheetId="0">#REF!</definedName>
@@ -43,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="333">
   <si>
     <t>fieldname</t>
   </si>
@@ -1116,6 +1113,18 @@
   </si>
   <si>
     <t>4 TCB</t>
+  </si>
+  <si>
+    <t>ASL_COLOUR [factor]</t>
+  </si>
+  <si>
+    <t>1. BLUE 2. BUFF/YELLOW 3. GREEN 4. NONE 5. OTHER 6. RED</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
   </si>
 </sst>
 </file>
@@ -1250,7 +1259,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1304,6 +1313,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1317,23 +1339,6 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Original_Schema"/>
-      <sheetName val="Asset Types"/>
-      <sheetName val="Fields"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1658,14 +1663,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1" enableFormatConditionsCalculation="0">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AG104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -1724,7 +1729,7 @@
       <c r="AF1" s="3"/>
       <c r="AG1" s="3"/>
     </row>
-    <row r="2" spans="1:33" ht="26" hidden="1" customHeight="1">
+    <row r="2" spans="1:33" ht="26" customHeight="1">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1737,8 +1742,12 @@
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="7"/>
+      <c r="E2" s="3">
+        <v>47.2</v>
+      </c>
+      <c r="F2" s="7">
+        <v>1783</v>
+      </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
@@ -1767,7 +1776,7 @@
       <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
     </row>
-    <row r="3" spans="1:33" ht="26" hidden="1" customHeight="1">
+    <row r="3" spans="1:33" ht="26" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>5</v>
       </c>
@@ -1780,8 +1789,12 @@
       <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="E3" s="3">
+        <v>44.9</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1695</v>
+      </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
       <c r="I3" s="3"/>
@@ -1810,7 +1823,7 @@
       <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
     </row>
-    <row r="4" spans="1:33" ht="26" hidden="1" customHeight="1">
+    <row r="4" spans="1:33" ht="26" customHeight="1">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1823,8 +1836,12 @@
       <c r="D4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="3">
+        <v>2.1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>78</v>
+      </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -1853,7 +1870,7 @@
       <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
     </row>
-    <row r="5" spans="1:33" ht="26" hidden="1" customHeight="1">
+    <row r="5" spans="1:33" ht="26" customHeight="1">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -1866,9 +1883,14 @@
       <c r="D5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E5"/>
-    </row>
-    <row r="6" spans="1:33" ht="26" hidden="1" customHeight="1">
+      <c r="E5" s="23">
+        <v>0.7</v>
+      </c>
+      <c r="F5" s="23">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" ht="26" customHeight="1">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1881,9 +1903,14 @@
       <c r="D6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E6"/>
-    </row>
-    <row r="7" spans="1:33" ht="26" hidden="1" customHeight="1">
+      <c r="E6" s="23">
+        <v>0.2</v>
+      </c>
+      <c r="F6" s="23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" ht="26" customHeight="1">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1898,7 +1925,7 @@
       </c>
       <c r="E7"/>
     </row>
-    <row r="8" spans="1:33" ht="26" hidden="1" customHeight="1">
+    <row r="8" spans="1:33" ht="26" customHeight="1">
       <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
@@ -1911,9 +1938,14 @@
       <c r="D8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E8"/>
-    </row>
-    <row r="9" spans="1:33" ht="26" hidden="1" customHeight="1">
+      <c r="E8" s="22">
+        <v>74.3</v>
+      </c>
+      <c r="F8">
+        <v>1254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" ht="26" customHeight="1">
       <c r="A9" s="5" t="s">
         <v>24</v>
       </c>
@@ -1926,9 +1958,14 @@
       <c r="D9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E9"/>
-    </row>
-    <row r="10" spans="1:33" ht="26" hidden="1" customHeight="1">
+      <c r="E9">
+        <v>18.899999999999999</v>
+      </c>
+      <c r="F9">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" ht="26" customHeight="1">
       <c r="A10" s="5" t="s">
         <v>24</v>
       </c>
@@ -1941,9 +1978,14 @@
       <c r="D10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E10"/>
-    </row>
-    <row r="11" spans="1:33" ht="26" hidden="1" customHeight="1">
+      <c r="E10">
+        <v>7.3</v>
+      </c>
+      <c r="F10">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" ht="26" customHeight="1">
       <c r="A11" s="5" t="s">
         <v>24</v>
       </c>
@@ -1956,9 +1998,14 @@
       <c r="D11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E11"/>
-    </row>
-    <row r="12" spans="1:33" ht="26" hidden="1" customHeight="1">
+      <c r="E11">
+        <v>2.5</v>
+      </c>
+      <c r="F11">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" ht="26" customHeight="1">
       <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
@@ -1971,7 +2018,12 @@
       <c r="D12" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="E12"/>
+      <c r="E12">
+        <v>1.2</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
     </row>
     <row r="13" spans="1:33" ht="26" customHeight="1">
       <c r="A13" s="5" t="s">
@@ -2310,7 +2362,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="26" hidden="1" customHeight="1">
+    <row r="30" spans="1:7" ht="26" customHeight="1">
       <c r="A30" s="5" t="s">
         <v>91</v>
       </c>
@@ -2325,7 +2377,7 @@
       </c>
       <c r="E30"/>
     </row>
-    <row r="31" spans="1:7" ht="26" hidden="1" customHeight="1">
+    <row r="31" spans="1:7" ht="26" customHeight="1">
       <c r="A31" s="5" t="s">
         <v>91</v>
       </c>
@@ -2340,7 +2392,7 @@
       </c>
       <c r="E31"/>
     </row>
-    <row r="32" spans="1:7" ht="26" hidden="1" customHeight="1">
+    <row r="32" spans="1:7" ht="26" customHeight="1">
       <c r="A32" s="5" t="s">
         <v>91</v>
       </c>
@@ -2355,7 +2407,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="33" spans="1:5" ht="26" customHeight="1">
       <c r="A33" s="5" t="s">
         <v>91</v>
       </c>
@@ -2370,7 +2422,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="34" spans="1:5" ht="26" customHeight="1">
       <c r="A34" s="5" t="s">
         <v>91</v>
       </c>
@@ -2385,7 +2437,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="35" spans="1:5" ht="26" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>91</v>
       </c>
@@ -2400,7 +2452,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="36" spans="1:5" ht="26" customHeight="1">
       <c r="A36" s="5" t="s">
         <v>91</v>
       </c>
@@ -2415,7 +2467,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="37" spans="1:5" ht="26" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>91</v>
       </c>
@@ -2430,7 +2482,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="38" spans="1:5" ht="26" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>91</v>
       </c>
@@ -2445,7 +2497,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="39" spans="1:5" ht="26" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>91</v>
       </c>
@@ -2460,7 +2512,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="40" spans="1:5" ht="26" customHeight="1">
       <c r="A40" s="5" t="s">
         <v>91</v>
       </c>
@@ -2475,7 +2527,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="41" spans="1:5" ht="26" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>91</v>
       </c>
@@ -2490,7 +2542,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="42" spans="1:5" ht="26" customHeight="1">
       <c r="A42" s="5" t="s">
         <v>91</v>
       </c>
@@ -2505,7 +2557,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="43" spans="1:5" ht="26" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>91</v>
       </c>
@@ -2520,7 +2572,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="44" spans="1:5" ht="26" customHeight="1">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -2535,7 +2587,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="45" spans="1:5" ht="26" customHeight="1">
       <c r="A45" s="5" t="s">
         <v>91</v>
       </c>
@@ -2550,7 +2602,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="46" spans="1:5" ht="26" customHeight="1">
       <c r="A46" s="15" t="s">
         <v>140</v>
       </c>
@@ -2565,7 +2617,7 @@
       </c>
       <c r="E46"/>
     </row>
-    <row r="47" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="47" spans="1:5" ht="26" customHeight="1">
       <c r="A47" s="15" t="s">
         <v>140</v>
       </c>
@@ -2580,7 +2632,7 @@
       </c>
       <c r="E47"/>
     </row>
-    <row r="48" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="48" spans="1:5" ht="26" customHeight="1">
       <c r="A48" s="5" t="s">
         <v>147</v>
       </c>
@@ -2595,7 +2647,7 @@
       </c>
       <c r="E48"/>
     </row>
-    <row r="49" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="49" spans="1:5" ht="26" customHeight="1">
       <c r="A49" s="5" t="s">
         <v>147</v>
       </c>
@@ -2610,7 +2662,7 @@
       </c>
       <c r="E49"/>
     </row>
-    <row r="50" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="50" spans="1:5" ht="26" customHeight="1">
       <c r="A50" s="5" t="s">
         <v>147</v>
       </c>
@@ -2625,7 +2677,7 @@
       </c>
       <c r="E50"/>
     </row>
-    <row r="51" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="51" spans="1:5" ht="26" customHeight="1">
       <c r="A51" s="5" t="s">
         <v>147</v>
       </c>
@@ -2640,7 +2692,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="52" spans="1:5" ht="26" customHeight="1">
       <c r="A52" s="5" t="s">
         <v>147</v>
       </c>
@@ -2655,7 +2707,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="53" spans="1:5" ht="26" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>161</v>
       </c>
@@ -2670,7 +2722,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="54" spans="1:5" ht="26" customHeight="1">
       <c r="A54" s="15" t="s">
         <v>161</v>
       </c>
@@ -2685,7 +2737,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="55" spans="1:5" ht="26" customHeight="1">
       <c r="A55" s="15" t="s">
         <v>161</v>
       </c>
@@ -2700,7 +2752,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="56" spans="1:5" ht="26" customHeight="1">
       <c r="A56" s="15" t="s">
         <v>161</v>
       </c>
@@ -2715,7 +2767,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="57" spans="1:5" ht="26" customHeight="1">
       <c r="A57" s="15" t="s">
         <v>161</v>
       </c>
@@ -2730,7 +2782,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="58" spans="1:5" ht="26" customHeight="1">
       <c r="A58" s="15" t="s">
         <v>161</v>
       </c>
@@ -2745,7 +2797,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="59" spans="1:5" ht="26" customHeight="1">
       <c r="A59" s="15" t="s">
         <v>161</v>
       </c>
@@ -2760,7 +2812,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="60" spans="1:5" ht="26" customHeight="1">
       <c r="A60" s="15" t="s">
         <v>161</v>
       </c>
@@ -2775,7 +2827,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="61" spans="1:5" ht="26" customHeight="1">
       <c r="A61" s="15" t="s">
         <v>161</v>
       </c>
@@ -2790,7 +2842,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="62" spans="1:5" ht="26" customHeight="1">
       <c r="A62" s="15" t="s">
         <v>161</v>
       </c>
@@ -2805,7 +2857,7 @@
       </c>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="63" spans="1:5" ht="26" customHeight="1">
       <c r="A63" s="15" t="s">
         <v>161</v>
       </c>
@@ -2820,7 +2872,7 @@
       </c>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="64" spans="1:5" ht="26" customHeight="1">
       <c r="A64" s="15" t="s">
         <v>161</v>
       </c>
@@ -2835,7 +2887,7 @@
       </c>
       <c r="E64"/>
     </row>
-    <row r="65" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="65" spans="1:5" ht="26" customHeight="1">
       <c r="A65" s="15" t="s">
         <v>161</v>
       </c>
@@ -2850,7 +2902,7 @@
       </c>
       <c r="E65"/>
     </row>
-    <row r="66" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="66" spans="1:5" ht="26" customHeight="1">
       <c r="A66" s="15" t="s">
         <v>161</v>
       </c>
@@ -2865,7 +2917,7 @@
       </c>
       <c r="E66"/>
     </row>
-    <row r="67" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="67" spans="1:5" ht="26" customHeight="1">
       <c r="A67" s="15" t="s">
         <v>161</v>
       </c>
@@ -2880,7 +2932,7 @@
       </c>
       <c r="E67"/>
     </row>
-    <row r="68" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="68" spans="1:5" ht="26" customHeight="1">
       <c r="A68" s="15" t="s">
         <v>161</v>
       </c>
@@ -2895,7 +2947,7 @@
       </c>
       <c r="E68"/>
     </row>
-    <row r="69" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="69" spans="1:5" ht="26" customHeight="1">
       <c r="A69" s="15" t="s">
         <v>161</v>
       </c>
@@ -2910,7 +2962,7 @@
       </c>
       <c r="E69"/>
     </row>
-    <row r="70" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="70" spans="1:5" ht="26" customHeight="1">
       <c r="A70" s="15" t="s">
         <v>161</v>
       </c>
@@ -2925,7 +2977,7 @@
       </c>
       <c r="E70"/>
     </row>
-    <row r="71" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="71" spans="1:5" ht="26" customHeight="1">
       <c r="A71" s="15" t="s">
         <v>161</v>
       </c>
@@ -2940,7 +2992,7 @@
       </c>
       <c r="E71"/>
     </row>
-    <row r="72" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="72" spans="1:5" ht="26" customHeight="1">
       <c r="A72" s="15" t="s">
         <v>161</v>
       </c>
@@ -2955,7 +3007,7 @@
       </c>
       <c r="E72"/>
     </row>
-    <row r="73" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="73" spans="1:5" ht="26" customHeight="1">
       <c r="A73" s="15" t="s">
         <v>161</v>
       </c>
@@ -2970,7 +3022,7 @@
       </c>
       <c r="E73"/>
     </row>
-    <row r="74" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="74" spans="1:5" ht="26" customHeight="1">
       <c r="A74" s="15" t="s">
         <v>161</v>
       </c>
@@ -2985,7 +3037,7 @@
       </c>
       <c r="E74"/>
     </row>
-    <row r="75" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="75" spans="1:5" ht="26" customHeight="1">
       <c r="A75" s="15" t="s">
         <v>161</v>
       </c>
@@ -3000,7 +3052,7 @@
       </c>
       <c r="E75"/>
     </row>
-    <row r="76" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="76" spans="1:5" ht="26" customHeight="1">
       <c r="A76" s="15" t="s">
         <v>161</v>
       </c>
@@ -3015,7 +3067,7 @@
       </c>
       <c r="E76"/>
     </row>
-    <row r="77" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="77" spans="1:5" ht="26" customHeight="1">
       <c r="A77" s="15" t="s">
         <v>161</v>
       </c>
@@ -3030,7 +3082,7 @@
       </c>
       <c r="E77"/>
     </row>
-    <row r="78" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="78" spans="1:5" ht="26" customHeight="1">
       <c r="A78" s="15" t="s">
         <v>161</v>
       </c>
@@ -3045,7 +3097,7 @@
       </c>
       <c r="E78"/>
     </row>
-    <row r="79" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="79" spans="1:5" ht="26" customHeight="1">
       <c r="A79" s="15" t="s">
         <v>161</v>
       </c>
@@ -3060,7 +3112,7 @@
       </c>
       <c r="E79"/>
     </row>
-    <row r="80" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="80" spans="1:5" ht="26" customHeight="1">
       <c r="A80" s="15" t="s">
         <v>161</v>
       </c>
@@ -3075,7 +3127,7 @@
       </c>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="81" spans="1:5" ht="26" customHeight="1">
       <c r="A81" s="15" t="s">
         <v>161</v>
       </c>
@@ -3090,7 +3142,7 @@
       </c>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="82" spans="1:5" ht="26" customHeight="1">
       <c r="A82" s="15" t="s">
         <v>161</v>
       </c>
@@ -3105,7 +3157,7 @@
       </c>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="83" spans="1:5" ht="26" customHeight="1">
       <c r="A83" s="15" t="s">
         <v>161</v>
       </c>
@@ -3120,7 +3172,7 @@
       </c>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="84" spans="1:5" ht="26" customHeight="1">
       <c r="A84" s="15" t="s">
         <v>253</v>
       </c>
@@ -3135,7 +3187,7 @@
       </c>
       <c r="E84"/>
     </row>
-    <row r="85" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="85" spans="1:5" ht="26" customHeight="1">
       <c r="A85" s="15" t="s">
         <v>253</v>
       </c>
@@ -3150,7 +3202,7 @@
       </c>
       <c r="E85"/>
     </row>
-    <row r="86" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="86" spans="1:5" ht="26" customHeight="1">
       <c r="A86" s="15" t="s">
         <v>253</v>
       </c>
@@ -3165,7 +3217,7 @@
       </c>
       <c r="E86"/>
     </row>
-    <row r="87" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="87" spans="1:5" ht="26" customHeight="1">
       <c r="A87" s="15" t="s">
         <v>253</v>
       </c>
@@ -3180,7 +3232,7 @@
       </c>
       <c r="E87"/>
     </row>
-    <row r="88" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="88" spans="1:5" ht="26" customHeight="1">
       <c r="A88" s="15" t="s">
         <v>253</v>
       </c>
@@ -3195,7 +3247,7 @@
       </c>
       <c r="E88"/>
     </row>
-    <row r="89" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="89" spans="1:5" ht="26" customHeight="1">
       <c r="A89" s="15" t="s">
         <v>269</v>
       </c>
@@ -3210,7 +3262,7 @@
       </c>
       <c r="E89"/>
     </row>
-    <row r="90" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="90" spans="1:5" ht="26" customHeight="1">
       <c r="A90" s="15" t="s">
         <v>269</v>
       </c>
@@ -3225,7 +3277,7 @@
       </c>
       <c r="E90"/>
     </row>
-    <row r="91" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="91" spans="1:5" ht="26" customHeight="1">
       <c r="A91" s="15" t="s">
         <v>269</v>
       </c>
@@ -3240,7 +3292,7 @@
       </c>
       <c r="E91"/>
     </row>
-    <row r="92" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="92" spans="1:5" ht="26" customHeight="1">
       <c r="A92" s="15" t="s">
         <v>269</v>
       </c>
@@ -3255,7 +3307,7 @@
       </c>
       <c r="E92"/>
     </row>
-    <row r="93" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="93" spans="1:5" ht="26" customHeight="1">
       <c r="A93" s="15" t="s">
         <v>269</v>
       </c>
@@ -3270,7 +3322,7 @@
       </c>
       <c r="E93"/>
     </row>
-    <row r="94" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="94" spans="1:5" ht="26" customHeight="1">
       <c r="A94" s="15" t="s">
         <v>269</v>
       </c>
@@ -3285,7 +3337,7 @@
       </c>
       <c r="E94"/>
     </row>
-    <row r="95" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="95" spans="1:5" ht="26" customHeight="1">
       <c r="A95" s="15" t="s">
         <v>269</v>
       </c>
@@ -3300,7 +3352,7 @@
       </c>
       <c r="E95"/>
     </row>
-    <row r="96" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="96" spans="1:5" ht="26" customHeight="1">
       <c r="A96" s="15" t="s">
         <v>269</v>
       </c>
@@ -3315,7 +3367,7 @@
       </c>
       <c r="E96"/>
     </row>
-    <row r="97" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="97" spans="1:5" ht="26" customHeight="1">
       <c r="A97" s="15"/>
       <c r="B97" s="11" t="s">
         <v>292</v>
@@ -3328,7 +3380,7 @@
       </c>
       <c r="E97"/>
     </row>
-    <row r="98" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="98" spans="1:5" ht="26" customHeight="1">
       <c r="A98" s="18"/>
       <c r="B98" s="11" t="s">
         <v>295</v>
@@ -3341,7 +3393,7 @@
       </c>
       <c r="E98"/>
     </row>
-    <row r="99" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="99" spans="1:5" ht="26" customHeight="1">
       <c r="A99" s="18"/>
       <c r="B99" s="11" t="s">
         <v>298</v>
@@ -3354,7 +3406,7 @@
       </c>
       <c r="E99"/>
     </row>
-    <row r="100" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="100" spans="1:5" ht="26" customHeight="1">
       <c r="A100" s="18"/>
       <c r="B100" s="11" t="s">
         <v>301</v>
@@ -3367,7 +3419,7 @@
       </c>
       <c r="E100"/>
     </row>
-    <row r="101" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="101" spans="1:5" ht="26" customHeight="1">
       <c r="A101" s="18"/>
       <c r="B101" s="11" t="s">
         <v>304</v>
@@ -3380,7 +3432,7 @@
       </c>
       <c r="E101"/>
     </row>
-    <row r="102" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="102" spans="1:5" ht="26" customHeight="1">
       <c r="A102" s="18"/>
       <c r="B102" s="11" t="s">
         <v>306</v>
@@ -3393,7 +3445,7 @@
       </c>
       <c r="E102"/>
     </row>
-    <row r="103" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="103" spans="1:5" ht="26" customHeight="1">
       <c r="A103" s="18"/>
       <c r="B103" s="11" t="s">
         <v>309</v>
@@ -3406,17 +3458,10 @@
       </c>
       <c r="E103"/>
     </row>
-    <row r="104" spans="1:5" ht="26" hidden="1" customHeight="1">
+    <row r="104" spans="1:5" ht="26" customHeight="1">
       <c r="E104"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E104">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Cycle Lane/Track"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait"/>
   <extLst>
@@ -3429,10 +3474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -3497,7 +3542,109 @@
         <v>326</v>
       </c>
     </row>
+    <row r="18" spans="1:6" ht="24" customHeight="1">
+      <c r="A18" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="C18" s="25">
+        <v>85</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="E18" s="26">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="27"/>
+      <c r="B19" s="27"/>
+      <c r="C19" s="25">
+        <v>21</v>
+      </c>
+      <c r="D19" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="E19" s="26">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F19" s="24" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="27"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="25">
+        <v>889</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="E20" s="26">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F20" s="24" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="27"/>
+      <c r="B21" s="27"/>
+      <c r="C21" s="25">
+        <v>2713</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="E21" s="26">
+        <v>0.71899999999999997</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="27"/>
+      <c r="B22" s="27"/>
+      <c r="C22" s="25">
+        <v>4</v>
+      </c>
+      <c r="D22" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="E22" s="26">
+        <v>1E-3</v>
+      </c>
+      <c r="F22" s="24" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="27"/>
+      <c r="B23" s="27"/>
+      <c r="C23" s="25">
+        <v>63</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>331</v>
+      </c>
+      <c r="E23" s="26">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F23" s="24"/>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A18:A23"/>
+    <mergeCell ref="B18:B23"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>

<commit_message>
lots of maps and more coding
</commit_message>
<xml_diff>
--- a/Results table.xlsx
+++ b/Results table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3500" yWindow="2200" windowWidth="27720" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="1180" yWindow="1200" windowWidth="27720" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$A$1:$E$104</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Fields!$B$1:$G$104</definedName>
     <definedName name="cons_day_rate" localSheetId="0">#REF!</definedName>
     <definedName name="cons_day_rate">#REF!</definedName>
     <definedName name="dayrate" localSheetId="0">#REF!</definedName>
@@ -1669,8 +1669,8 @@
   <dimension ref="A1:AG104"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A78" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D87" sqref="D87"/>
+      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E89" sqref="E89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2059,7 +2059,7 @@
         <v>45</v>
       </c>
       <c r="E14" s="22">
-        <v>7.68</v>
+        <v>7.7</v>
       </c>
       <c r="F14">
         <v>1917</v>
@@ -2079,7 +2079,7 @@
         <v>48</v>
       </c>
       <c r="E15" s="22">
-        <v>0.42</v>
+        <v>0.4</v>
       </c>
       <c r="F15">
         <v>104</v>
@@ -2142,7 +2142,7 @@
         <v>57</v>
       </c>
       <c r="E18" s="22">
-        <v>7.37</v>
+        <v>7.4</v>
       </c>
       <c r="F18">
         <v>1841</v>
@@ -2165,7 +2165,7 @@
         <v>60</v>
       </c>
       <c r="E19" s="22">
-        <v>28.91</v>
+        <v>28.9</v>
       </c>
       <c r="F19">
         <v>7221</v>
@@ -2185,7 +2185,7 @@
         <v>63</v>
       </c>
       <c r="E20" s="22">
-        <v>9.06</v>
+        <v>9.1</v>
       </c>
       <c r="F20">
         <v>2264</v>
@@ -2208,7 +2208,7 @@
         <v>66</v>
       </c>
       <c r="E21" s="22">
-        <v>5.97</v>
+        <v>6</v>
       </c>
       <c r="F21">
         <v>1490</v>
@@ -2228,7 +2228,7 @@
         <v>69</v>
       </c>
       <c r="E22" s="22">
-        <v>40.89</v>
+        <v>40.9</v>
       </c>
       <c r="F22">
         <v>10213</v>
@@ -2248,7 +2248,7 @@
         <v>72</v>
       </c>
       <c r="E23" s="22">
-        <v>0.25</v>
+        <v>0.2</v>
       </c>
       <c r="F23">
         <v>63</v>
@@ -2268,7 +2268,7 @@
         <v>75</v>
       </c>
       <c r="E24" s="22">
-        <v>0.53</v>
+        <v>0.5</v>
       </c>
       <c r="F24">
         <v>132</v>
@@ -2288,7 +2288,7 @@
         <v>78</v>
       </c>
       <c r="E25" s="22">
-        <v>16.28</v>
+        <v>16.3</v>
       </c>
       <c r="F25">
         <v>4067</v>
@@ -2308,7 +2308,7 @@
         <v>81</v>
       </c>
       <c r="E26" s="22">
-        <v>2.29</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F26">
         <v>573</v>
@@ -2407,7 +2407,7 @@
       </c>
       <c r="E32"/>
     </row>
-    <row r="33" spans="1:5" ht="26" customHeight="1">
+    <row r="33" spans="1:6" ht="26" customHeight="1">
       <c r="A33" s="5" t="s">
         <v>91</v>
       </c>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="E33"/>
     </row>
-    <row r="34" spans="1:5" ht="26" customHeight="1">
+    <row r="34" spans="1:6" ht="26" customHeight="1">
       <c r="A34" s="5" t="s">
         <v>91</v>
       </c>
@@ -2437,7 +2437,7 @@
       </c>
       <c r="E34"/>
     </row>
-    <row r="35" spans="1:5" ht="26" customHeight="1">
+    <row r="35" spans="1:6" ht="26" customHeight="1">
       <c r="A35" s="5" t="s">
         <v>91</v>
       </c>
@@ -2452,7 +2452,7 @@
       </c>
       <c r="E35"/>
     </row>
-    <row r="36" spans="1:5" ht="26" customHeight="1">
+    <row r="36" spans="1:6" ht="26" customHeight="1">
       <c r="A36" s="5" t="s">
         <v>91</v>
       </c>
@@ -2467,7 +2467,7 @@
       </c>
       <c r="E36"/>
     </row>
-    <row r="37" spans="1:5" ht="26" customHeight="1">
+    <row r="37" spans="1:6" ht="26" customHeight="1">
       <c r="A37" s="5" t="s">
         <v>91</v>
       </c>
@@ -2482,7 +2482,7 @@
       </c>
       <c r="E37"/>
     </row>
-    <row r="38" spans="1:5" ht="26" customHeight="1">
+    <row r="38" spans="1:6" ht="26" customHeight="1">
       <c r="A38" s="5" t="s">
         <v>91</v>
       </c>
@@ -2497,7 +2497,7 @@
       </c>
       <c r="E38"/>
     </row>
-    <row r="39" spans="1:5" ht="26" customHeight="1">
+    <row r="39" spans="1:6" ht="26" customHeight="1">
       <c r="A39" s="5" t="s">
         <v>91</v>
       </c>
@@ -2512,7 +2512,7 @@
       </c>
       <c r="E39"/>
     </row>
-    <row r="40" spans="1:5" ht="26" customHeight="1">
+    <row r="40" spans="1:6" ht="26" customHeight="1">
       <c r="A40" s="5" t="s">
         <v>91</v>
       </c>
@@ -2527,7 +2527,7 @@
       </c>
       <c r="E40"/>
     </row>
-    <row r="41" spans="1:5" ht="26" customHeight="1">
+    <row r="41" spans="1:6" ht="26" customHeight="1">
       <c r="A41" s="5" t="s">
         <v>91</v>
       </c>
@@ -2542,7 +2542,7 @@
       </c>
       <c r="E41"/>
     </row>
-    <row r="42" spans="1:5" ht="26" customHeight="1">
+    <row r="42" spans="1:6" ht="26" customHeight="1">
       <c r="A42" s="5" t="s">
         <v>91</v>
       </c>
@@ -2557,7 +2557,7 @@
       </c>
       <c r="E42"/>
     </row>
-    <row r="43" spans="1:5" ht="26" customHeight="1">
+    <row r="43" spans="1:6" ht="26" customHeight="1">
       <c r="A43" s="5" t="s">
         <v>91</v>
       </c>
@@ -2572,7 +2572,7 @@
       </c>
       <c r="E43"/>
     </row>
-    <row r="44" spans="1:5" ht="26" customHeight="1">
+    <row r="44" spans="1:6" ht="26" customHeight="1">
       <c r="A44" s="5" t="s">
         <v>91</v>
       </c>
@@ -2587,7 +2587,7 @@
       </c>
       <c r="E44"/>
     </row>
-    <row r="45" spans="1:5" ht="26" customHeight="1">
+    <row r="45" spans="1:6" ht="26" customHeight="1">
       <c r="A45" s="5" t="s">
         <v>91</v>
       </c>
@@ -2602,7 +2602,7 @@
       </c>
       <c r="E45"/>
     </row>
-    <row r="46" spans="1:5" ht="26" customHeight="1">
+    <row r="46" spans="1:6" ht="26" customHeight="1">
       <c r="A46" s="15" t="s">
         <v>140</v>
       </c>
@@ -2615,9 +2615,14 @@
       <c r="D46" s="4" t="s">
         <v>142</v>
       </c>
-      <c r="E46"/>
-    </row>
-    <row r="47" spans="1:5" ht="26" customHeight="1">
+      <c r="E46">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F46">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="26" customHeight="1">
       <c r="A47" s="15" t="s">
         <v>140</v>
       </c>
@@ -2630,9 +2635,14 @@
       <c r="D47" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="E47"/>
-    </row>
-    <row r="48" spans="1:5" ht="26" customHeight="1">
+      <c r="E47">
+        <v>0.1</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="26" customHeight="1">
       <c r="A48" s="5" t="s">
         <v>147</v>
       </c>
@@ -2645,9 +2655,14 @@
       <c r="D48" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="E48"/>
-    </row>
-    <row r="49" spans="1:5" ht="26" customHeight="1">
+      <c r="E48">
+        <v>99.7</v>
+      </c>
+      <c r="F48">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="26" customHeight="1">
       <c r="A49" s="5" t="s">
         <v>147</v>
       </c>
@@ -2660,9 +2675,14 @@
       <c r="D49" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="E49"/>
-    </row>
-    <row r="50" spans="1:5" ht="26" customHeight="1">
+      <c r="E49">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F49">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="26" customHeight="1">
       <c r="A50" s="5" t="s">
         <v>147</v>
       </c>
@@ -2675,9 +2695,14 @@
       <c r="D50" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="E50"/>
-    </row>
-    <row r="51" spans="1:5" ht="26" customHeight="1">
+      <c r="E50">
+        <v>4.3</v>
+      </c>
+      <c r="F50">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="26" customHeight="1">
       <c r="A51" s="5" t="s">
         <v>147</v>
       </c>
@@ -2692,7 +2717,7 @@
       </c>
       <c r="E51"/>
     </row>
-    <row r="52" spans="1:5" ht="26" customHeight="1">
+    <row r="52" spans="1:6" ht="26" customHeight="1">
       <c r="A52" s="5" t="s">
         <v>147</v>
       </c>
@@ -2707,7 +2732,7 @@
       </c>
       <c r="E52"/>
     </row>
-    <row r="53" spans="1:5" ht="26" customHeight="1">
+    <row r="53" spans="1:6" ht="26" customHeight="1">
       <c r="A53" s="15" t="s">
         <v>161</v>
       </c>
@@ -2722,7 +2747,7 @@
       </c>
       <c r="E53"/>
     </row>
-    <row r="54" spans="1:5" ht="26" customHeight="1">
+    <row r="54" spans="1:6" ht="26" customHeight="1">
       <c r="A54" s="15" t="s">
         <v>161</v>
       </c>
@@ -2737,7 +2762,7 @@
       </c>
       <c r="E54"/>
     </row>
-    <row r="55" spans="1:5" ht="26" customHeight="1">
+    <row r="55" spans="1:6" ht="26" customHeight="1">
       <c r="A55" s="15" t="s">
         <v>161</v>
       </c>
@@ -2752,7 +2777,7 @@
       </c>
       <c r="E55"/>
     </row>
-    <row r="56" spans="1:5" ht="26" customHeight="1">
+    <row r="56" spans="1:6" ht="26" customHeight="1">
       <c r="A56" s="15" t="s">
         <v>161</v>
       </c>
@@ -2767,7 +2792,7 @@
       </c>
       <c r="E56"/>
     </row>
-    <row r="57" spans="1:5" ht="26" customHeight="1">
+    <row r="57" spans="1:6" ht="26" customHeight="1">
       <c r="A57" s="15" t="s">
         <v>161</v>
       </c>
@@ -2782,7 +2807,7 @@
       </c>
       <c r="E57"/>
     </row>
-    <row r="58" spans="1:5" ht="26" customHeight="1">
+    <row r="58" spans="1:6" ht="26" customHeight="1">
       <c r="A58" s="15" t="s">
         <v>161</v>
       </c>
@@ -2797,7 +2822,7 @@
       </c>
       <c r="E58"/>
     </row>
-    <row r="59" spans="1:5" ht="26" customHeight="1">
+    <row r="59" spans="1:6" ht="26" customHeight="1">
       <c r="A59" s="15" t="s">
         <v>161</v>
       </c>
@@ -2812,7 +2837,7 @@
       </c>
       <c r="E59"/>
     </row>
-    <row r="60" spans="1:5" ht="26" customHeight="1">
+    <row r="60" spans="1:6" ht="26" customHeight="1">
       <c r="A60" s="15" t="s">
         <v>161</v>
       </c>
@@ -2827,7 +2852,7 @@
       </c>
       <c r="E60"/>
     </row>
-    <row r="61" spans="1:5" ht="26" customHeight="1">
+    <row r="61" spans="1:6" ht="26" customHeight="1">
       <c r="A61" s="15" t="s">
         <v>161</v>
       </c>
@@ -2842,7 +2867,7 @@
       </c>
       <c r="E61"/>
     </row>
-    <row r="62" spans="1:5" ht="26" customHeight="1">
+    <row r="62" spans="1:6" ht="26" customHeight="1">
       <c r="A62" s="15" t="s">
         <v>161</v>
       </c>
@@ -2857,7 +2882,7 @@
       </c>
       <c r="E62"/>
     </row>
-    <row r="63" spans="1:5" ht="26" customHeight="1">
+    <row r="63" spans="1:6" ht="26" customHeight="1">
       <c r="A63" s="15" t="s">
         <v>161</v>
       </c>
@@ -2872,7 +2897,7 @@
       </c>
       <c r="E63"/>
     </row>
-    <row r="64" spans="1:5" ht="26" customHeight="1">
+    <row r="64" spans="1:6" ht="26" customHeight="1">
       <c r="A64" s="15" t="s">
         <v>161</v>
       </c>
@@ -3127,7 +3152,7 @@
       </c>
       <c r="E80"/>
     </row>
-    <row r="81" spans="1:5" ht="26" customHeight="1">
+    <row r="81" spans="1:6" ht="26" customHeight="1">
       <c r="A81" s="15" t="s">
         <v>161</v>
       </c>
@@ -3142,7 +3167,7 @@
       </c>
       <c r="E81"/>
     </row>
-    <row r="82" spans="1:5" ht="26" customHeight="1">
+    <row r="82" spans="1:6" ht="26" customHeight="1">
       <c r="A82" s="15" t="s">
         <v>161</v>
       </c>
@@ -3157,7 +3182,7 @@
       </c>
       <c r="E82"/>
     </row>
-    <row r="83" spans="1:5" ht="26" customHeight="1">
+    <row r="83" spans="1:6" ht="26" customHeight="1">
       <c r="A83" s="15" t="s">
         <v>161</v>
       </c>
@@ -3172,7 +3197,7 @@
       </c>
       <c r="E83"/>
     </row>
-    <row r="84" spans="1:5" ht="26" customHeight="1">
+    <row r="84" spans="1:6" ht="26" customHeight="1">
       <c r="A84" s="15" t="s">
         <v>253</v>
       </c>
@@ -3185,9 +3210,14 @@
       <c r="D84" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="E84"/>
-    </row>
-    <row r="85" spans="1:5" ht="26" customHeight="1">
+      <c r="E84">
+        <v>98.9</v>
+      </c>
+      <c r="F84">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" ht="26" customHeight="1">
       <c r="A85" s="15" t="s">
         <v>253</v>
       </c>
@@ -3200,9 +3230,14 @@
       <c r="D85" s="4" t="s">
         <v>258</v>
       </c>
-      <c r="E85"/>
-    </row>
-    <row r="86" spans="1:5" ht="26" customHeight="1">
+      <c r="E85">
+        <v>57.8</v>
+      </c>
+      <c r="F85">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" ht="26" customHeight="1">
       <c r="A86" s="15" t="s">
         <v>253</v>
       </c>
@@ -3215,9 +3250,14 @@
       <c r="D86" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="E86"/>
-    </row>
-    <row r="87" spans="1:5" ht="26" customHeight="1">
+      <c r="E86">
+        <v>18.100000000000001</v>
+      </c>
+      <c r="F86">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" ht="26" customHeight="1">
       <c r="A87" s="15" t="s">
         <v>253</v>
       </c>
@@ -3230,9 +3270,14 @@
       <c r="D87" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="E87"/>
-    </row>
-    <row r="88" spans="1:5" ht="26" customHeight="1">
+      <c r="E87">
+        <v>6.3</v>
+      </c>
+      <c r="F87">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" ht="26" customHeight="1">
       <c r="A88" s="15" t="s">
         <v>253</v>
       </c>
@@ -3245,9 +3290,14 @@
       <c r="D88" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="E88"/>
-    </row>
-    <row r="89" spans="1:5" ht="26" customHeight="1">
+      <c r="E88">
+        <v>6.3</v>
+      </c>
+      <c r="F88">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" ht="26" customHeight="1">
       <c r="A89" s="15" t="s">
         <v>269</v>
       </c>
@@ -3262,7 +3312,7 @@
       </c>
       <c r="E89"/>
     </row>
-    <row r="90" spans="1:5" ht="26" customHeight="1">
+    <row r="90" spans="1:6" ht="26" customHeight="1">
       <c r="A90" s="15" t="s">
         <v>269</v>
       </c>
@@ -3277,7 +3327,7 @@
       </c>
       <c r="E90"/>
     </row>
-    <row r="91" spans="1:5" ht="26" customHeight="1">
+    <row r="91" spans="1:6" ht="26" customHeight="1">
       <c r="A91" s="15" t="s">
         <v>269</v>
       </c>
@@ -3292,7 +3342,7 @@
       </c>
       <c r="E91"/>
     </row>
-    <row r="92" spans="1:5" ht="26" customHeight="1">
+    <row r="92" spans="1:6" ht="26" customHeight="1">
       <c r="A92" s="15" t="s">
         <v>269</v>
       </c>
@@ -3307,7 +3357,7 @@
       </c>
       <c r="E92"/>
     </row>
-    <row r="93" spans="1:5" ht="26" customHeight="1">
+    <row r="93" spans="1:6" ht="26" customHeight="1">
       <c r="A93" s="15" t="s">
         <v>269</v>
       </c>
@@ -3322,7 +3372,7 @@
       </c>
       <c r="E93"/>
     </row>
-    <row r="94" spans="1:5" ht="26" customHeight="1">
+    <row r="94" spans="1:6" ht="26" customHeight="1">
       <c r="A94" s="15" t="s">
         <v>269</v>
       </c>
@@ -3337,7 +3387,7 @@
       </c>
       <c r="E94"/>
     </row>
-    <row r="95" spans="1:5" ht="26" customHeight="1">
+    <row r="95" spans="1:6" ht="26" customHeight="1">
       <c r="A95" s="15" t="s">
         <v>269</v>
       </c>
@@ -3352,7 +3402,7 @@
       </c>
       <c r="E95"/>
     </row>
-    <row r="96" spans="1:5" ht="26" customHeight="1">
+    <row r="96" spans="1:6" ht="26" customHeight="1">
       <c r="A96" s="15" t="s">
         <v>269</v>
       </c>
@@ -3462,6 +3512,7 @@
       <c r="E104"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:G104"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait"/>
   <extLst>

</xml_diff>

<commit_message>
more maps for points
</commit_message>
<xml_diff>
--- a/Results table.xlsx
+++ b/Results table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28028"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5000" yWindow="1420" windowWidth="27720" windowHeight="14720" tabRatio="500"/>
+    <workbookView xWindow="4660" yWindow="1700" windowWidth="27720" windowHeight="14720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Fields" sheetId="1" r:id="rId1"/>
@@ -24,6 +24,7 @@
     <definedName name="Notes" localSheetId="0">#REF!</definedName>
     <definedName name="Notes">#REF!</definedName>
     <definedName name="Notes2">#REF!</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Fields!$A$1:$G$103</definedName>
     <definedName name="sdas2">#REF!</definedName>
     <definedName name="sdasdsa" localSheetId="0">#REF!</definedName>
     <definedName name="sdasdsa">#REF!</definedName>
@@ -1134,7 +1135,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1193,6 +1194,10 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -1675,9 +1680,9 @@
   </sheetPr>
   <dimension ref="A1:AG104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A99" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A108" sqref="A108"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2836,7 +2841,12 @@
       <c r="D53" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E53"/>
+      <c r="E53">
+        <v>50.9</v>
+      </c>
+      <c r="F53">
+        <v>60484</v>
+      </c>
     </row>
     <row r="54" spans="1:6" ht="26" customHeight="1">
       <c r="A54" s="15" t="s">
@@ -2851,7 +2861,12 @@
       <c r="D54" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="E54"/>
+      <c r="E54">
+        <v>1.5</v>
+      </c>
+      <c r="F54">
+        <v>1721</v>
+      </c>
     </row>
     <row r="55" spans="1:6" ht="26" customHeight="1">
       <c r="A55" s="15" t="s">
@@ -2881,7 +2896,12 @@
       <c r="D56" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="E56"/>
+      <c r="E56">
+        <v>14.6</v>
+      </c>
+      <c r="F56">
+        <v>17389</v>
+      </c>
     </row>
     <row r="57" spans="1:6" ht="26" customHeight="1">
       <c r="A57" s="15" t="s">
@@ -2896,7 +2916,12 @@
       <c r="D57" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="E57"/>
+      <c r="E57">
+        <v>10.3</v>
+      </c>
+      <c r="F57">
+        <v>12240</v>
+      </c>
     </row>
     <row r="58" spans="1:6" ht="26" customHeight="1">
       <c r="A58" s="15" t="s">
@@ -2911,7 +2936,12 @@
       <c r="D58" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E58"/>
+      <c r="E58">
+        <v>0.2</v>
+      </c>
+      <c r="F58">
+        <v>272</v>
+      </c>
     </row>
     <row r="59" spans="1:6" ht="26" customHeight="1">
       <c r="A59" s="15" t="s">
@@ -2926,7 +2956,12 @@
       <c r="D59" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E59"/>
+      <c r="E59">
+        <v>25</v>
+      </c>
+      <c r="F59">
+        <v>29693</v>
+      </c>
     </row>
     <row r="60" spans="1:6" ht="26" customHeight="1">
       <c r="A60" s="15" t="s">
@@ -2941,7 +2976,12 @@
       <c r="D60" s="4" t="s">
         <v>184</v>
       </c>
-      <c r="E60"/>
+      <c r="E60">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="F60">
+        <v>2716</v>
+      </c>
     </row>
     <row r="61" spans="1:6" ht="26" customHeight="1">
       <c r="A61" s="15" t="s">
@@ -2956,7 +2996,12 @@
       <c r="D61" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="E61"/>
+      <c r="E61">
+        <v>0.2</v>
+      </c>
+      <c r="F61">
+        <v>234</v>
+      </c>
     </row>
     <row r="62" spans="1:6" ht="26" customHeight="1">
       <c r="A62" s="15" t="s">
@@ -2971,7 +3016,12 @@
       <c r="D62" s="4" t="s">
         <v>190</v>
       </c>
-      <c r="E62"/>
+      <c r="E62">
+        <v>0.2</v>
+      </c>
+      <c r="F62">
+        <v>301</v>
+      </c>
     </row>
     <row r="63" spans="1:6" ht="26" customHeight="1">
       <c r="A63" s="15" t="s">
@@ -2986,7 +3036,12 @@
       <c r="D63" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E63"/>
+      <c r="E63">
+        <v>0.2</v>
+      </c>
+      <c r="F63">
+        <v>255</v>
+      </c>
     </row>
     <row r="64" spans="1:6" ht="26" customHeight="1">
       <c r="A64" s="15" t="s">
@@ -3001,9 +3056,14 @@
       <c r="D64" s="4" t="s">
         <v>196</v>
       </c>
-      <c r="E64"/>
-    </row>
-    <row r="65" spans="1:5" ht="26" customHeight="1">
+      <c r="E64">
+        <v>0.1</v>
+      </c>
+      <c r="F64">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="26" customHeight="1">
       <c r="A65" s="15" t="s">
         <v>161</v>
       </c>
@@ -3016,9 +3076,14 @@
       <c r="D65" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="E65"/>
-    </row>
-    <row r="66" spans="1:5" ht="26" customHeight="1">
+      <c r="E65">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F65">
+        <v>2661</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="26" customHeight="1">
       <c r="A66" s="15" t="s">
         <v>161</v>
       </c>
@@ -3031,9 +3096,14 @@
       <c r="D66" s="4" t="s">
         <v>202</v>
       </c>
-      <c r="E66"/>
-    </row>
-    <row r="67" spans="1:5" ht="26" customHeight="1">
+      <c r="E66">
+        <v>0.7</v>
+      </c>
+      <c r="F66">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" ht="26" customHeight="1">
       <c r="A67" s="15" t="s">
         <v>161</v>
       </c>
@@ -3046,9 +3116,14 @@
       <c r="D67" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E67"/>
-    </row>
-    <row r="68" spans="1:5" ht="26" customHeight="1">
+      <c r="E67">
+        <v>0.2</v>
+      </c>
+      <c r="F67">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="26" customHeight="1">
       <c r="A68" s="15" t="s">
         <v>161</v>
       </c>
@@ -3061,9 +3136,14 @@
       <c r="D68" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="E68"/>
-    </row>
-    <row r="69" spans="1:5" ht="26" customHeight="1">
+      <c r="E68">
+        <v>95.6</v>
+      </c>
+      <c r="F68">
+        <v>113654</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" ht="26" customHeight="1">
       <c r="A69" s="15" t="s">
         <v>161</v>
       </c>
@@ -3076,9 +3156,14 @@
       <c r="D69" s="4" t="s">
         <v>211</v>
       </c>
-      <c r="E69"/>
-    </row>
-    <row r="70" spans="1:5" ht="26" customHeight="1">
+      <c r="E69">
+        <v>14.3</v>
+      </c>
+      <c r="F69">
+        <v>17057</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" ht="26" customHeight="1">
       <c r="A70" s="15" t="s">
         <v>161</v>
       </c>
@@ -3091,9 +3176,14 @@
       <c r="D70" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="E70"/>
-    </row>
-    <row r="71" spans="1:5" ht="26" customHeight="1">
+      <c r="E70">
+        <v>3.1</v>
+      </c>
+      <c r="F70">
+        <v>3712</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="26" customHeight="1">
       <c r="A71" s="15" t="s">
         <v>161</v>
       </c>
@@ -3106,9 +3196,14 @@
       <c r="D71" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="E71"/>
-    </row>
-    <row r="72" spans="1:5" ht="26" customHeight="1">
+      <c r="E71">
+        <v>3.7</v>
+      </c>
+      <c r="F71">
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" ht="26" customHeight="1">
       <c r="A72" s="15" t="s">
         <v>161</v>
       </c>
@@ -3121,9 +3216,14 @@
       <c r="D72" s="4" t="s">
         <v>220</v>
       </c>
-      <c r="E72"/>
-    </row>
-    <row r="73" spans="1:5" ht="26" customHeight="1">
+      <c r="E72">
+        <v>3.6</v>
+      </c>
+      <c r="F72">
+        <v>4243</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" ht="26" customHeight="1">
       <c r="A73" s="15" t="s">
         <v>161</v>
       </c>
@@ -3136,9 +3236,14 @@
       <c r="D73" s="4" t="s">
         <v>223</v>
       </c>
-      <c r="E73"/>
-    </row>
-    <row r="74" spans="1:5" ht="26" customHeight="1">
+      <c r="E73">
+        <v>1.2</v>
+      </c>
+      <c r="F73">
+        <v>1441</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" ht="26" customHeight="1">
       <c r="A74" s="15" t="s">
         <v>161</v>
       </c>
@@ -3151,9 +3256,14 @@
       <c r="D74" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="E74"/>
-    </row>
-    <row r="75" spans="1:5" ht="26" customHeight="1">
+      <c r="E74">
+        <v>8.5</v>
+      </c>
+      <c r="F74">
+        <v>10143</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" ht="26" customHeight="1">
       <c r="A75" s="15" t="s">
         <v>161</v>
       </c>
@@ -3166,9 +3276,14 @@
       <c r="D75" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E75"/>
-    </row>
-    <row r="76" spans="1:5" ht="26" customHeight="1">
+      <c r="E75">
+        <v>2.9</v>
+      </c>
+      <c r="F75">
+        <v>3472</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" ht="26" customHeight="1">
       <c r="A76" s="15" t="s">
         <v>161</v>
       </c>
@@ -3181,9 +3296,14 @@
       <c r="D76" s="4" t="s">
         <v>232</v>
       </c>
-      <c r="E76"/>
-    </row>
-    <row r="77" spans="1:5" ht="26" customHeight="1">
+      <c r="E76">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="F76">
+        <v>10442</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" ht="26" customHeight="1">
       <c r="A77" s="15" t="s">
         <v>161</v>
       </c>
@@ -3196,9 +3316,14 @@
       <c r="D77" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="E77"/>
-    </row>
-    <row r="78" spans="1:5" ht="26" customHeight="1">
+      <c r="E77">
+        <v>2.1</v>
+      </c>
+      <c r="F77">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" ht="26" customHeight="1">
       <c r="A78" s="15" t="s">
         <v>161</v>
       </c>
@@ -3211,9 +3336,14 @@
       <c r="D78" s="4" t="s">
         <v>238</v>
       </c>
-      <c r="E78"/>
-    </row>
-    <row r="79" spans="1:5" ht="26" customHeight="1">
+      <c r="E78">
+        <v>1.2</v>
+      </c>
+      <c r="F78">
+        <v>1470</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" ht="26" customHeight="1">
       <c r="A79" s="15" t="s">
         <v>161</v>
       </c>
@@ -3226,9 +3356,14 @@
       <c r="D79" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="E79"/>
-    </row>
-    <row r="80" spans="1:5" ht="26" customHeight="1">
+      <c r="E79">
+        <v>0.2</v>
+      </c>
+      <c r="F79">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" ht="26" customHeight="1">
       <c r="A80" s="15" t="s">
         <v>161</v>
       </c>
@@ -3256,7 +3391,12 @@
       <c r="D81" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E81"/>
+      <c r="E81">
+        <v>12.2</v>
+      </c>
+      <c r="F81">
+        <v>14456</v>
+      </c>
     </row>
     <row r="82" spans="1:6" ht="26" customHeight="1">
       <c r="A82" s="15" t="s">
@@ -3401,7 +3541,12 @@
       <c r="D89" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="E89"/>
+      <c r="E89">
+        <v>4.7</v>
+      </c>
+      <c r="F89">
+        <v>2772</v>
+      </c>
     </row>
     <row r="90" spans="1:6" ht="26" customHeight="1">
       <c r="A90" s="15" t="s">
@@ -3416,7 +3561,12 @@
       <c r="D90" s="6" t="s">
         <v>274</v>
       </c>
-      <c r="E90"/>
+      <c r="E90">
+        <v>12.9</v>
+      </c>
+      <c r="F90">
+        <v>7581</v>
+      </c>
     </row>
     <row r="91" spans="1:6" ht="26" customHeight="1">
       <c r="A91" s="15" t="s">
@@ -3431,7 +3581,12 @@
       <c r="D91" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="E91"/>
+      <c r="E91">
+        <v>21.6</v>
+      </c>
+      <c r="F91">
+        <v>12626</v>
+      </c>
     </row>
     <row r="92" spans="1:6" ht="26" customHeight="1">
       <c r="A92" s="15" t="s">
@@ -3446,7 +3601,12 @@
       <c r="D92" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="E92"/>
+      <c r="E92">
+        <v>56.8</v>
+      </c>
+      <c r="F92">
+        <v>33271</v>
+      </c>
     </row>
     <row r="93" spans="1:6" ht="26" customHeight="1">
       <c r="A93" s="15" t="s">
@@ -3461,7 +3621,12 @@
       <c r="D93" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="E93"/>
+      <c r="E93">
+        <v>11.5</v>
+      </c>
+      <c r="F93">
+        <v>6720</v>
+      </c>
     </row>
     <row r="94" spans="1:6" ht="26" customHeight="1">
       <c r="A94" s="15" t="s">
@@ -3476,7 +3641,12 @@
       <c r="D94" s="6" t="s">
         <v>286</v>
       </c>
-      <c r="E94"/>
+      <c r="E94">
+        <v>1.6</v>
+      </c>
+      <c r="F94">
+        <v>935</v>
+      </c>
     </row>
     <row r="95" spans="1:6" ht="26" customHeight="1">
       <c r="A95" s="15" t="s">
@@ -3491,7 +3661,12 @@
       <c r="D95" s="13" t="s">
         <v>289</v>
       </c>
-      <c r="E95"/>
+      <c r="E95">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F95">
+        <v>662</v>
+      </c>
     </row>
     <row r="96" spans="1:6" ht="26" customHeight="1">
       <c r="A96" s="15" t="s">
@@ -3506,7 +3681,12 @@
       <c r="D96" s="6" t="s">
         <v>291</v>
       </c>
-      <c r="E96"/>
+      <c r="E96">
+        <v>1.2</v>
+      </c>
+      <c r="F96">
+        <v>721</v>
+      </c>
     </row>
     <row r="97" spans="1:5" ht="26" customHeight="1">
       <c r="A97" s="15"/>
@@ -3603,9 +3783,9 @@
       <c r="E104"/>
     </row>
   </sheetData>
-  <autoFilter ref="B1:G104"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="44" orientation="portrait"/>
+  <phoneticPr fontId="10" type="noConversion"/>
+  <pageMargins left="0.70000000000000007" right="0.70000000000000007" top="0.75000000000000011" bottom="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+  <pageSetup paperSize="9" scale="68" fitToHeight="5" orientation="landscape"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>